<commit_message>
0.51: Updated PLC logic
</commit_message>
<xml_diff>
--- a/_Assets/FD.xlsx
+++ b/_Assets/FD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\TwinCAT\Punch1\Punch\_Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8238C525-5418-4FA9-AD0B-ED37218BAD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B942B07-4AB3-44B9-A234-A0B48C363A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23040" yWindow="1644" windowWidth="14748" windowHeight="10716" tabRatio="776" activeTab="5" xr2:uid="{0C0DCA5D-D4EA-4B89-800E-6027767AA106}"/>
+    <workbookView minimized="1" xWindow="23040" yWindow="1644" windowWidth="14748" windowHeight="10716" tabRatio="776" activeTab="5" xr2:uid="{0C0DCA5D-D4EA-4B89-800E-6027767AA106}"/>
   </bookViews>
   <sheets>
     <sheet name="Safeties" sheetId="2" r:id="rId1"/>
@@ -745,7 +745,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344C23B6-C141-402D-93F5-CAA796CBD1F8}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
0.54: Completed Overview Page
</commit_message>
<xml_diff>
--- a/_Assets/FD.xlsx
+++ b/_Assets/FD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\TwinCAT\Punch1\Punch\_Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B942B07-4AB3-44B9-A234-A0B48C363A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328F626D-0340-48CD-A86A-70A6F58875CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="23040" yWindow="1644" windowWidth="14748" windowHeight="10716" tabRatio="776" activeTab="5" xr2:uid="{0C0DCA5D-D4EA-4B89-800E-6027767AA106}"/>
+    <workbookView xWindow="23760" yWindow="1500" windowWidth="16224" windowHeight="10716" tabRatio="776" firstSheet="1" activeTab="1" xr2:uid="{0C0DCA5D-D4EA-4B89-800E-6027767AA106}"/>
   </bookViews>
   <sheets>
     <sheet name="Safeties" sheetId="2" r:id="rId1"/>
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC23CFE-EB3B-495D-9462-9904A6991081}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,7 +874,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344C23B6-C141-402D-93F5-CAA796CBD1F8}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
@@ -1305,12 +1305,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e7c3118f-7fae-4a88-908f-add9ecbff707" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="62d6d6c5-65e1-4014-a8f3-e6ca1c548838">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1569,20 +1571,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e7c3118f-7fae-4a88-908f-add9ecbff707" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="62d6d6c5-65e1-4014-a8f3-e6ca1c548838">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19BEB324-AAA4-46DF-A0B4-62F3AA5877AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{561A7291-B743-48CD-BFE3-69CD013EB4BA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7c3118f-7fae-4a88-908f-add9ecbff707"/>
+    <ds:schemaRef ds:uri="62d6d6c5-65e1-4014-a8f3-e6ca1c548838"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1607,12 +1610,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{561A7291-B743-48CD-BFE3-69CD013EB4BA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19BEB324-AAA4-46DF-A0B4-62F3AA5877AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7c3118f-7fae-4a88-908f-add9ecbff707"/>
-    <ds:schemaRef ds:uri="62d6d6c5-65e1-4014-a8f3-e6ca1c548838"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>